<commit_message>
upload questionnaire answers without coloration
</commit_message>
<xml_diff>
--- a/data/participant_questionnaire_answers.xlsx
+++ b/data/participant_questionnaire_answers.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanja\Documents\master\msc_repo\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tanja\Documents\master\MSc\MSc\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA8988E-1A6A-4943-AFE1-120280FDFAA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{119D3308-6B05-4FD2-B8EE-47248F830C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{0D173897-CC3E-40DA-ADEC-B60B74C2D35F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="292">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="260">
   <si>
     <t>Dataset</t>
   </si>
@@ -749,75 +749,6 @@
     <t>20, 25</t>
   </si>
   <si>
-    <t>Focus on the goal and bring the object to the goal</t>
-  </si>
-  <si>
-    <t>see the object try to estimate it and then remember this goal point from before</t>
-  </si>
-  <si>
-    <t>i comare the estimation with the size of disc while performing</t>
-  </si>
-  <si>
-    <t>judgement based on initival viewin go the disc</t>
-  </si>
-  <si>
-    <t>try to remember the size of object seen and compare to the shown one</t>
-  </si>
-  <si>
-    <t>i think 2; i don't think the amount of discs change</t>
-  </si>
-  <si>
-    <t>12, 15</t>
-  </si>
-  <si>
-    <t>Breite ungefähr gemerkt nach Gefühl in Fingern abgeschätzt, wenn ich das Gefühl hatte, da war zu viel Abweichung habe ich es angepasst.</t>
-  </si>
-  <si>
-    <t>direkt mit manueller Einschätzung verglichen</t>
-  </si>
-  <si>
-    <t>4; nicht verändert</t>
-  </si>
-  <si>
-    <t>25, 30, 35, 37.5</t>
-  </si>
-  <si>
-    <t>Notfalls den letzten Teil blind machen</t>
-  </si>
-  <si>
-    <t>Anhand der Betrachtung</t>
-  </si>
-  <si>
-    <t>6; ich glaube, am Ende wurden es weniger. Scheibengröße hat sich gefühlt kaum mehr verändert.</t>
-  </si>
-  <si>
-    <t>(40-50) 38, 40, 41, 44, 47, 48</t>
-  </si>
-  <si>
-    <t>38, 40, 41, 44, 47, 48</t>
-  </si>
-  <si>
-    <t>Die Hand auf dem Bildschirm lassen für mehr Kontrolle und nur die Finger heben</t>
-  </si>
-  <si>
-    <t>gleiche Strategie wie oben.</t>
-  </si>
-  <si>
-    <t>mal so, mal so</t>
-  </si>
-  <si>
-    <t>mit den Scheiben davor verglichen aber eher einfach nach Gefühl</t>
-  </si>
-  <si>
-    <t>7, keine Veränderung gemerkt</t>
-  </si>
-  <si>
-    <t>(24mm) 21, 22, 23, 24, 25, 26, 27</t>
-  </si>
-  <si>
-    <t>21, 22, 23, 24, 25, 26, 27</t>
-  </si>
-  <si>
     <t>No specfific strategy. Tried to mark (note: not sure it says "mark") and estimate as well as possible.</t>
   </si>
   <si>
@@ -866,30 +797,6 @@
     <t>lots of manest practice</t>
   </si>
   <si>
-    <t>Give enough attention to the object and last position of it given that I felt that I had more time to do the task</t>
-  </si>
-  <si>
-    <t>I estimated based on my initial view of the disc.</t>
-  </si>
-  <si>
-    <t>First I saw the disc in the right and second I started seeing the left one because I felt that my first observation gave more volumen to the object</t>
-  </si>
-  <si>
-    <t>While performing</t>
-  </si>
-  <si>
-    <t>No particular strategy</t>
-  </si>
-  <si>
-    <t>I assume I had to distinguish between 2 sizes. They were alterenated during the experiment.</t>
-  </si>
-  <si>
-    <t>44, 45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Give less attention to the left side and focus on the center and right side; I considered 2 seconds was not enough to see all the 3 points so I prioritised seeing just the center and the right. So I did the first estimation more mechanic while given more attention to move the disc in the right position. </t>
-  </si>
-  <si>
     <t>super fast reaction time doing ex/perc, but claimed was still doing task correctly; visual acuity left eye was 0.35 &amp; 0.18</t>
   </si>
   <si>
@@ -906,9 +813,6 @@
   </si>
   <si>
     <t>Tried to reemeber the last one shown. Sometimes compared it to "SAMSUNG" (note: written on monitor on experimenter's side); compared to relative size of previous disc shown.</t>
-  </si>
-  <si>
-    <t>dreimal Scheibe gewechselt, die ich angeschaut hab und dann entschieden welche größer wirkt (note: image with left, right, left)</t>
   </si>
   <si>
     <t>30, 30.25</t>
@@ -927,7 +831,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -936,25 +840,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.34998626667073579"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -988,7 +874,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -997,27 +883,18 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1025,6 +902,15 @@
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="none">
@@ -1053,9 +939,12 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1068,24 +957,66 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
       <alignment horizontal="general" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1105,21 +1036,21 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{70A6DAF9-B808-4697-9677-D4DAC2591668}" name="Tabelle1" displayName="Tabelle1" ref="A1:L38" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A1:L38" xr:uid="{70A6DAF9-B808-4697-9677-D4DAC2591668}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{70A6DAF9-B808-4697-9677-D4DAC2591668}" name="Tabelle1" displayName="Tabelle1" ref="A1:L33" totalsRowShown="0" headerRowDxfId="13" dataDxfId="0">
+  <autoFilter ref="A1:L33" xr:uid="{70A6DAF9-B808-4697-9677-D4DAC2591668}"/>
   <tableColumns count="12">
-    <tableColumn id="1" xr3:uid="{B6CB2506-B796-4582-B320-0B089CE9F882}" name="Dataset" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{C018E55D-3B85-4374-926E-E5F0D027716F}" name="Group" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{36C5C2F3-0C0F-4AD2-8873-05211F3ED37B}" name="Grasp Strat" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{38747460-8AC4-4A08-8B3D-0CFF3218F2A7}" name="ManEst Strat" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{7365643B-50A1-4A53-8BE6-518980CAC64D}" name="ManEst Order" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{5F9EF76E-0B4B-4C47-A84B-00DCB30DD55D}" name="Perc Strat" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{53587D1F-8C2C-441D-8212-9C43C25B4E92}" name="Perc Order" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{33BF177A-EBEC-4511-A6D3-718BFC65A8D3}" name="ExPerc Strat" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{D1E2D6CD-6057-446D-8BCE-B5C74B9424BD}" name="General" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{6C74A2D0-E72D-45A4-9077-5C6D705AC698}" name="General Sizes" dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{F51DF14A-5270-4AD9-929B-E158B8629850}" name="General Sizes clean" dataDxfId="1"/>
-    <tableColumn id="12" xr3:uid="{9F6847E9-5AA7-48C0-B730-84F72384DB1D}" name="Relevant conduction notes" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{B6CB2506-B796-4582-B320-0B089CE9F882}" name="Dataset" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{C018E55D-3B85-4374-926E-E5F0D027716F}" name="Group" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{36C5C2F3-0C0F-4AD2-8873-05211F3ED37B}" name="Grasp Strat" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{38747460-8AC4-4A08-8B3D-0CFF3218F2A7}" name="ManEst Strat" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{7365643B-50A1-4A53-8BE6-518980CAC64D}" name="ManEst Order" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{5F9EF76E-0B4B-4C47-A84B-00DCB30DD55D}" name="Perc Strat" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{53587D1F-8C2C-441D-8212-9C43C25B4E92}" name="Perc Order" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{33BF177A-EBEC-4511-A6D3-718BFC65A8D3}" name="ExPerc Strat" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{D1E2D6CD-6057-446D-8BCE-B5C74B9424BD}" name="General" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{6C74A2D0-E72D-45A4-9077-5C6D705AC698}" name="General Sizes" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{F51DF14A-5270-4AD9-929B-E158B8629850}" name="General Sizes clean" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{9F6847E9-5AA7-48C0-B730-84F72384DB1D}" name="Relevant conduction notes" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1442,10 +1373,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82686E09-7DFD-4CDF-8D41-BA39E118ABB7}">
-  <dimension ref="A1:L38"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34:XFD38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1466,145 +1397,145 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>271</v>
+        <v>248</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>272</v>
+        <v>249</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>273</v>
+        <v>250</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>270</v>
+        <v>247</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>269</v>
+        <v>246</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>268</v>
+        <v>245</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>267</v>
+        <v>244</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>266</v>
+        <v>243</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>265</v>
+        <v>242</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>264</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="1">
+      <c r="A2" s="5">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
+      <c r="C2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="J2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="2" t="s">
-        <v>291</v>
-      </c>
-      <c r="L2" s="2"/>
+      <c r="K2" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="L2" s="6"/>
     </row>
     <row r="3" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A3" s="1">
+      <c r="A3" s="5">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="2" t="s">
+      <c r="C3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="J3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="K3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="L3" s="2"/>
+      <c r="L3" s="6"/>
     </row>
     <row r="4" spans="1:12" ht="57" x14ac:dyDescent="0.45">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
+      <c r="A4" s="5">
+        <v>3</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="7" t="s">
+      <c r="C4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="F4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I4" s="2" t="s">
+      <c r="H4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="J4" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="K4" s="2" t="s">
+      <c r="K4" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="L4" s="2"/>
-    </row>
-    <row r="5" spans="1:12" s="5" customFormat="1" ht="213.75" x14ac:dyDescent="0.45">
+      <c r="L4" s="6"/>
+    </row>
+    <row r="5" spans="1:12" s="3" customFormat="1" ht="213.75" x14ac:dyDescent="0.45">
       <c r="A5" s="5">
         <v>4</v>
       </c>
@@ -1641,836 +1572,836 @@
       <c r="L5" s="6"/>
     </row>
     <row r="6" spans="1:12" ht="199.5" x14ac:dyDescent="0.45">
-      <c r="A6" s="1">
+      <c r="A6" s="5">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="G6" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="H6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="J6" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="K6" s="2">
+      <c r="K6" s="6">
         <v>45</v>
       </c>
-      <c r="L6" s="2"/>
+      <c r="L6" s="6"/>
     </row>
     <row r="7" spans="1:12" ht="114" x14ac:dyDescent="0.45">
-      <c r="A7" s="1">
+      <c r="A7" s="5">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="C7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G7" s="2" t="s">
+      <c r="F7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="7" t="s">
+      <c r="H7" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="8" t="s">
+      <c r="I7" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="J7" s="7" t="s">
+      <c r="J7" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="K7" s="7" t="s">
+      <c r="K7" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="L7" s="2"/>
+      <c r="L7" s="6"/>
     </row>
     <row r="8" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A8" s="1">
+      <c r="A8" s="5">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D8" s="7" t="s">
+      <c r="C8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G8" s="2" t="s">
+      <c r="F8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I8" s="2" t="s">
+      <c r="H8" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I8" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="J8" s="2" t="s">
+      <c r="J8" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="K8" s="2" t="s">
+      <c r="K8" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="L8" s="2"/>
+      <c r="L8" s="6"/>
     </row>
     <row r="9" spans="1:12" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A9" s="1">
+      <c r="A9" s="5">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="G9" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="H9" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="J9" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="K9" s="6" t="s">
         <v>153</v>
       </c>
-      <c r="L9" s="2"/>
+      <c r="L9" s="6"/>
     </row>
     <row r="10" spans="1:12" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="A10" s="1">
+      <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="E10" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="G10" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="H10" s="7" t="s">
+      <c r="H10" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="J10" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="L10" s="2"/>
+      <c r="L10" s="6"/>
     </row>
     <row r="11" spans="1:12" ht="114" x14ac:dyDescent="0.45">
-      <c r="A11" s="1">
+      <c r="A11" s="5">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="C11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="E11" s="7" t="s">
+      <c r="E11" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="G11" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="H11" s="7" t="s">
+      <c r="H11" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="J11" s="6" t="s">
         <v>75</v>
       </c>
-      <c r="K11" s="2" t="s">
+      <c r="K11" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="L11" s="2"/>
+      <c r="L11" s="6"/>
     </row>
     <row r="12" spans="1:12" ht="128.25" x14ac:dyDescent="0.45">
-      <c r="A12" s="1">
+      <c r="A12" s="5">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="G12" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="H12" s="7" t="s">
+      <c r="H12" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="J12" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="K12" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="L12" s="2"/>
+      <c r="L12" s="6"/>
     </row>
     <row r="13" spans="1:12" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A13" s="1">
+      <c r="A13" s="5">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="G13" s="2" t="s">
+      <c r="G13" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="H13" s="2" t="s">
+      <c r="H13" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="I13" s="8" t="s">
+      <c r="I13" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J13" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="K13" s="2">
+      <c r="K13" s="6">
         <v>30</v>
       </c>
-      <c r="L13" s="2"/>
+      <c r="L13" s="6"/>
     </row>
     <row r="14" spans="1:12" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A14" s="1">
+      <c r="A14" s="5">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="E14" s="2" t="s">
+      <c r="D14" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="E14" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="G14" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="H14" s="6" t="s">
         <v>98</v>
       </c>
-      <c r="I14" s="8" t="s">
+      <c r="I14" s="6" t="s">
         <v>99</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="J14" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="K14" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="L14" s="2"/>
-    </row>
-    <row r="15" spans="1:12" s="9" customFormat="1" ht="128.25" x14ac:dyDescent="0.45">
-      <c r="A15" s="9">
+      <c r="L14" s="6"/>
+    </row>
+    <row r="15" spans="1:12" s="4" customFormat="1" ht="128.25" x14ac:dyDescent="0.45">
+      <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="6" t="s">
         <v>101</v>
       </c>
-      <c r="D15" s="10" t="s">
-        <v>261</v>
-      </c>
-      <c r="E15" s="10" t="s">
+      <c r="D15" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>102</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H15" s="6" t="s">
         <v>105</v>
       </c>
-      <c r="I15" s="10" t="s">
+      <c r="I15" s="6" t="s">
         <v>106</v>
       </c>
-      <c r="J15" s="10" t="s">
+      <c r="J15" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="K15" s="10" t="s">
+      <c r="K15" s="6" t="s">
         <v>158</v>
       </c>
-      <c r="L15" s="10"/>
+      <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:12" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A16" s="1">
+      <c r="A16" s="5">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="6" t="s">
         <v>107</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G16" s="2" t="s">
+      <c r="F16" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="6" t="s">
         <v>110</v>
       </c>
-      <c r="H16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I16" s="7" t="s">
+      <c r="H16" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I16" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="J16" s="6" t="s">
         <v>112</v>
       </c>
-      <c r="K16" s="2">
+      <c r="K16" s="6">
         <v>30</v>
       </c>
-      <c r="L16" s="2"/>
-    </row>
-    <row r="17" spans="1:12" s="9" customFormat="1" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A17" s="9">
+      <c r="L16" s="6"/>
+    </row>
+    <row r="17" spans="1:12" s="4" customFormat="1" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="A17" s="5">
         <v>16</v>
       </c>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C17" s="10" t="s">
+      <c r="C17" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="D17" s="10" t="s">
+      <c r="D17" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="E17" s="10" t="s">
+      <c r="E17" s="6" t="s">
         <v>116</v>
       </c>
-      <c r="F17" s="10" t="s">
-        <v>286</v>
-      </c>
-      <c r="G17" s="10" t="s">
+      <c r="F17" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="G17" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="H17" s="10" t="s">
+      <c r="H17" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="I17" s="10" t="s">
+      <c r="I17" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="6">
         <v>4</v>
       </c>
-      <c r="K17" s="10">
+      <c r="K17" s="6">
         <v>4</v>
       </c>
-      <c r="L17" s="10"/>
+      <c r="L17" s="6"/>
     </row>
     <row r="18" spans="1:12" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A18" s="1">
+      <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="6" t="s">
         <v>120</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D18" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="E18" s="2" t="s">
+      <c r="E18" s="6" t="s">
         <v>122</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="F18" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="G18" s="6" t="s">
         <v>125</v>
       </c>
-      <c r="H18" s="7" t="s">
+      <c r="H18" s="6" t="s">
         <v>124</v>
       </c>
-      <c r="I18" s="7" t="s">
+      <c r="I18" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" s="6">
         <v>60</v>
       </c>
-      <c r="K18" s="2">
+      <c r="K18" s="6">
         <v>60</v>
       </c>
-      <c r="L18" s="2"/>
+      <c r="L18" s="6"/>
     </row>
     <row r="19" spans="1:12" ht="114" x14ac:dyDescent="0.45">
-      <c r="A19" s="1">
+      <c r="A19" s="5">
         <v>18</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="E19" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="G19" s="2" t="s">
+      <c r="G19" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="H19" s="2" t="s">
+      <c r="H19" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="J19" s="2" t="s">
+      <c r="J19" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="K19" s="2" t="s">
+      <c r="K19" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="L19" s="2"/>
+      <c r="L19" s="6"/>
     </row>
     <row r="20" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A20" s="1">
+      <c r="A20" s="5">
         <v>19</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>136</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="E20" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="F20" s="2" t="s">
+      <c r="F20" s="6" t="s">
         <v>138</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="H20" s="7" t="s">
+      <c r="H20" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="I20" s="2" t="s">
+      <c r="I20" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="J20" s="2" t="s">
+      <c r="J20" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="K20" s="2" t="s">
+      <c r="K20" s="6" t="s">
         <v>159</v>
       </c>
-      <c r="L20" s="2"/>
+      <c r="L20" s="6"/>
     </row>
     <row r="21" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A21" s="1">
+      <c r="A21" s="5">
         <v>20</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="6" t="s">
         <v>145</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="6" t="s">
         <v>146</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G21" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="H21" s="2" t="s">
+      <c r="H21" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="I21" s="2" t="s">
+      <c r="I21" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="J21" s="6" t="s">
         <v>150</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="K21" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="L21" s="2"/>
+      <c r="L21" s="6"/>
     </row>
     <row r="22" spans="1:12" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="A22" s="1">
+      <c r="A22" s="5">
         <v>21</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="B22" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="6" t="s">
         <v>161</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="6" t="s">
         <v>162</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="F22" s="2" t="s">
+      <c r="E22" s="6" t="s">
+        <v>256</v>
+      </c>
+      <c r="F22" s="6" t="s">
         <v>163</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G22" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="H22" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="I22" s="7" t="s">
+      <c r="H22" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="I22" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="J22" s="2" t="s">
+      <c r="J22" s="6" t="s">
         <v>166</v>
       </c>
-      <c r="K22" s="2" t="s">
+      <c r="K22" s="6" t="s">
         <v>167</v>
       </c>
-      <c r="L22" s="2" t="s">
-        <v>274</v>
+      <c r="L22" s="6" t="s">
+        <v>251</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A23" s="1">
+      <c r="A23" s="5">
         <v>22</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="7" t="s">
+      <c r="C23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D23" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="E23" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="F23" s="6" t="s">
         <v>170</v>
       </c>
-      <c r="G23" s="2" t="s">
+      <c r="G23" s="6" t="s">
         <v>171</v>
       </c>
-      <c r="H23" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I23" s="2" t="s">
+      <c r="H23" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I23" s="6" t="s">
         <v>172</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J23" s="6">
         <v>27</v>
       </c>
-      <c r="K23" s="2">
+      <c r="K23" s="6">
         <v>27</v>
       </c>
-      <c r="L23" s="2"/>
+      <c r="L23" s="6"/>
     </row>
     <row r="24" spans="1:12" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A24" s="1">
+      <c r="A24" s="5">
         <v>23</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="D24" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="E24" s="6" t="s">
         <v>175</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="G24" s="2" t="s">
+      <c r="G24" s="6" t="s">
         <v>177</v>
       </c>
-      <c r="H24" s="2" t="s">
+      <c r="H24" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="I24" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="J24" s="2" t="s">
+      <c r="I24" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="J24" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="K24" s="2" t="s">
+      <c r="K24" s="6" t="s">
         <v>179</v>
       </c>
-      <c r="L24" s="2"/>
+      <c r="L24" s="6"/>
     </row>
     <row r="25" spans="1:12" ht="57" x14ac:dyDescent="0.45">
-      <c r="A25" s="1">
+      <c r="A25" s="5">
         <v>24</v>
       </c>
-      <c r="B25" s="1" t="s">
+      <c r="B25" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="6" t="s">
         <v>181</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="F25" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="G25" s="2" t="s">
+      <c r="G25" s="6" t="s">
         <v>185</v>
       </c>
-      <c r="H25" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I25" s="2" t="s">
+      <c r="H25" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I25" s="6" t="s">
         <v>186</v>
       </c>
-      <c r="J25" s="2" t="s">
+      <c r="J25" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="K25" s="2" t="s">
+      <c r="K25" s="6" t="s">
         <v>134</v>
       </c>
-      <c r="L25" s="2"/>
+      <c r="L25" s="6"/>
     </row>
     <row r="26" spans="1:12" ht="185.25" x14ac:dyDescent="0.45">
-      <c r="A26" s="1">
+      <c r="A26" s="5">
         <v>25</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="B26" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C26" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="D26" s="7" t="s">
+      <c r="C26" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>187</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E26" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F26" s="6" t="s">
         <v>189</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G26" s="6" t="s">
         <v>190</v>
       </c>
-      <c r="H26" s="7" t="s">
+      <c r="H26" s="6" t="s">
         <v>191</v>
       </c>
-      <c r="I26" s="2" t="s">
+      <c r="I26" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="J26" s="2" t="s">
+      <c r="J26" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="K26" s="2" t="s">
+      <c r="K26" s="6" t="s">
         <v>193</v>
       </c>
-      <c r="L26" s="2"/>
+      <c r="L26" s="6"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A27" s="1">
+      <c r="A27" s="5">
         <v>26</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="B27" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E27" s="2" t="s">
+      <c r="C27" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="F27" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G27" s="2" t="s">
+      <c r="F27" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="H27" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I27" s="2" t="s">
+      <c r="H27" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="J27" s="2" t="s">
+      <c r="J27" s="6" t="s">
         <v>196</v>
       </c>
-      <c r="K27" s="2" t="s">
+      <c r="K27" s="6" t="s">
         <v>160</v>
       </c>
-      <c r="L27" s="2"/>
+      <c r="L27" s="6"/>
     </row>
     <row r="28" spans="1:12" ht="128.25" x14ac:dyDescent="0.45">
-      <c r="A28" s="1">
+      <c r="A28" s="5">
         <v>27</v>
       </c>
-      <c r="B28" s="1" t="s">
+      <c r="B28" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C28" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="6" t="s">
         <v>198</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="F28" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G28" s="2" t="s">
+      <c r="F28" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="H28" s="7" t="s">
-        <v>289</v>
-      </c>
-      <c r="I28" s="2" t="s">
+      <c r="H28" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="I28" s="6" t="s">
         <v>201</v>
       </c>
-      <c r="J28" s="2" t="s">
+      <c r="J28" s="6" t="s">
         <v>202</v>
       </c>
-      <c r="K28" s="2" t="s">
+      <c r="K28" s="6" t="s">
         <v>203</v>
       </c>
-      <c r="L28" s="2"/>
-    </row>
-    <row r="29" spans="1:12" s="5" customFormat="1" ht="156.75" x14ac:dyDescent="0.45">
+      <c r="L28" s="6"/>
+    </row>
+    <row r="29" spans="1:12" s="3" customFormat="1" ht="156.75" x14ac:dyDescent="0.45">
       <c r="A29" s="5">
         <v>28</v>
       </c>
@@ -2505,48 +2436,48 @@
         <v>50</v>
       </c>
       <c r="L29" s="6" t="s">
-        <v>284</v>
+        <v>253</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A30" s="1">
+      <c r="A30" s="5">
         <v>29</v>
       </c>
-      <c r="B30" s="1" t="s">
+      <c r="B30" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="6" t="s">
         <v>209</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="F30" s="8" t="s">
+      <c r="F30" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="G30" s="2" t="s">
+      <c r="G30" s="6" t="s">
         <v>213</v>
       </c>
-      <c r="H30" s="2" t="s">
+      <c r="H30" s="6" t="s">
         <v>214</v>
       </c>
-      <c r="I30" s="2" t="s">
+      <c r="I30" s="6" t="s">
         <v>215</v>
       </c>
-      <c r="J30" s="2" t="s">
+      <c r="J30" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="K30" s="2" t="s">
+      <c r="K30" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="L30" s="2" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" s="5" customFormat="1" ht="114" x14ac:dyDescent="0.45">
+      <c r="L30" s="6" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" s="3" customFormat="1" ht="114" x14ac:dyDescent="0.45">
       <c r="A31" s="5">
         <v>30</v>
       </c>
@@ -2583,258 +2514,78 @@
       <c r="L31" s="6"/>
     </row>
     <row r="32" spans="1:12" ht="114" x14ac:dyDescent="0.45">
-      <c r="A32" s="1">
+      <c r="A32" s="5">
         <v>31</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="D32" s="7" t="s">
+      <c r="D32" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="E32" s="2" t="s">
+      <c r="E32" s="6" t="s">
         <v>225</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G32" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="H32" s="2" t="s">
+      <c r="H32" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="I32" s="2" t="s">
+      <c r="I32" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="J32" s="2" t="s">
+      <c r="J32" s="6" t="s">
         <v>229</v>
       </c>
-      <c r="K32" s="2" t="s">
+      <c r="K32" s="6" t="s">
         <v>230</v>
       </c>
-      <c r="L32" s="2" t="s">
-        <v>285</v>
+      <c r="L32" s="6" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="185.25" x14ac:dyDescent="0.45">
-      <c r="A33" s="1">
+      <c r="A33" s="5">
         <v>32</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="6" t="s">
         <v>231</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="D33" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="E33" s="2" t="s">
+      <c r="E33" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="F33" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G33" s="2" t="s">
+      <c r="F33" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="G33" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="H33" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I33" s="2" t="s">
+      <c r="H33" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="I33" s="6" t="s">
         <v>234</v>
       </c>
-      <c r="J33" s="2" t="s">
+      <c r="J33" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="K33" s="2" t="s">
+      <c r="K33" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="L33" s="2"/>
-    </row>
-    <row r="34" spans="1:12" ht="57" x14ac:dyDescent="0.45">
-      <c r="A34" s="1">
-        <v>33</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>238</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="F34" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>240</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>241</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="J34" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="L34" s="2"/>
-    </row>
-    <row r="35" spans="1:12" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="A35" s="1">
-        <v>34</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C35" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="F35" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="J35" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="L35" s="2"/>
-    </row>
-    <row r="36" spans="1:12" ht="71.25" x14ac:dyDescent="0.45">
-      <c r="A36" s="1">
-        <v>35</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>248</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="F36" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="J36" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="L36" s="2"/>
-    </row>
-    <row r="37" spans="1:12" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="A37" s="1">
-        <v>36</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="G37" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="L37" s="2"/>
-    </row>
-    <row r="38" spans="1:12" ht="199.5" x14ac:dyDescent="0.45">
-      <c r="A38" s="1">
-        <v>37</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="D38" s="7" t="s">
-        <v>283</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>277</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="J38" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>282</v>
-      </c>
-      <c r="L38" s="2"/>
+      <c r="L33" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -3016,20 +2767,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d4ea612e-41eb-4b35-90ac-1df9ac331fe0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d4ea612e-41eb-4b35-90ac-1df9ac331fe0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3051,14 +2802,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BE04F61-3782-4A92-8010-820D535B819F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1E08488-5570-4774-A8DD-4393F9017F01}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -3072,4 +2815,12 @@
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1BE04F61-3782-4A92-8010-820D535B819F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>